<commit_message>
last commit of the night
</commit_message>
<xml_diff>
--- a/data/Exempel_case_allra.xlsx
+++ b/data/Exempel_case_allra.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="101">
   <si>
     <t xml:space="preserve">event</t>
   </si>
@@ -56,7 +56,10 @@
     <t xml:space="preserve">mobil2</t>
   </si>
   <si>
-    <t xml:space="preserve">Allra beslutar om utdelning</t>
+    <t xml:space="preserve">Allra beslutar om utdelning, kan misstänkas för penningtvätt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.svd.se/allra-utreds-for-misstankt-penningtvatt</t>
   </si>
   <si>
     <t xml:space="preserve">Styrelsen godkänner utdelning via dotterbolag I dubai</t>
@@ -95,30 +98,33 @@
     <t xml:space="preserve">url(#ernstberger)</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.di.se/nyheter/allras-grundare-begars-haktad/</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kronofogden säkrar tillgångar</t>
   </si>
   <si>
     <t xml:space="preserve">url(#kronofogden)</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.svd.se/kronofogden-fryser-miljoner-pa-ernstbergers-konton</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ernstberger köper landets dyraste villa år 2016</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.affarsvarlden.se/bostad-fastighet/allras-vd-alexander-ernstberger-kopte-dyraste-villan-2016-6817070</t>
+  </si>
+  <si>
     <t xml:space="preserve">Oak capital tar 40 % </t>
   </si>
   <si>
     <t xml:space="preserve">url(#oak)</t>
   </si>
   <si>
-    <t xml:space="preserve">2012-05</t>
-  </si>
-  <si>
     <t xml:space="preserve">mobil6</t>
   </si>
   <si>
-    <t xml:space="preserve">Allra startar dotterbolag i dubai</t>
-  </si>
-  <si>
     <t xml:space="preserve">Lindsö avgår från allras styrelse på allras årsstämma</t>
   </si>
   <si>
@@ -143,16 +149,16 @@
     <t xml:space="preserve">url(#svd)</t>
   </si>
   <si>
-    <t xml:space="preserve">Allra köper prognosia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">url(#prognosia)</t>
+    <t xml:space="preserve">https://www.svd.se/sparare-bortdribblade-i-det-kandistata-pensionsbolaget</t>
   </si>
   <si>
     <t xml:space="preserve">Allra polisanmäls av revisor</t>
   </si>
   <si>
-    <t xml:space="preserve">url(#revisor)</t>
+    <t xml:space="preserve">url(#deloitte)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.svd.se/pensionsmyndigheten-kommenterar-allra--svd-bevakar-live</t>
   </si>
   <si>
     <t xml:space="preserve">Allra polisanmäls av pensionsmyndigheten</t>
@@ -161,6 +167,9 @@
     <t xml:space="preserve">url(#pensionsmyndigheten)</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.svd.se/fem-personer-polisanmals-for-allra-skandalen</t>
+  </si>
+  <si>
     <t xml:space="preserve">PM beslutar om avregistrering</t>
   </si>
   <si>
@@ -170,6 +179,9 @@
     <t xml:space="preserve">Allra överklagar</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.svt.se/nyheter/inrikes/allra-kan-inte-overklaga</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kammarrätten stoppar avregistrering</t>
   </si>
   <si>
@@ -207,6 +219,57 @@
   </si>
   <si>
     <t xml:space="preserve">Bodström lämnar allras styrelse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.svd.se/just-nu-aven-thomas-bodstrom-lamnar-allra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lindsö lämnar SBABs styrelse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.svd.se/ebba-lindso-lamnar-styrelsen-i-sbab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22 000 sparare har lämnat allra sedan granskningen inleddes I SvD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.svd.se/flykten-fran-allra-fortsatter--miljarder-flodar-ut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uppgifter om Allras affärer med Oak capital kommer fram I SvD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.svd.se/fler-hoppar-av-allras-styrelse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Styrelseproffset Meg Tivéus lämnar Allras styrelse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.svd.se/fler-styrelseledamoter-flyr-allra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 PPM miljarder flyttade från Allras fonder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.svd.se/spararna-flyr-fran-allra--saljer-for-2-miljarder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allra chefer knutna till norsk skandal från 2013, Oak Capital</t>
+  </si>
+  <si>
+    <t xml:space="preserve">url(#norge)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.svd.se/tre-ppm-toppar-inblandade-i-norsk-finansskandal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ernstberger vägrar svara på frågor om nyttan med bolaget I Dubai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">url(#dubai)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.svd.se/ppm-bjassens-hemliga-bolag-i-skatteparadiset</t>
   </si>
   <si>
     <t xml:space="preserve">person</t>
@@ -629,10 +692,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D65536"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -699,10 +762,16 @@
       <c r="B5" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="C5" s="1" t="n">
+        <v>42969</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>9</v>
@@ -711,271 +780,403 @@
         <v>42671</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>42972</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>43022</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>42860</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>43020</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>43026</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>42677</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>41044</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>9</v>
+        <v>35</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>42822</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>42822</v>
+        <v>42775</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="0" t="s">
-        <v>33</v>
-      </c>
       <c r="C16" s="1" t="n">
-        <v>42775</v>
+        <v>42829</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>42829</v>
+        <v>42765</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>39</v>
+        <v>44</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>42810</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>41</v>
+        <v>47</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>42815</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>42816</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>45</v>
+        <v>9</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>42814</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>42816</v>
+        <v>42821</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>9</v>
+        <v>47</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>42780</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>42821</v>
+        <v>42898</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C25" s="1" t="n">
-        <v>42780</v>
+        <v>42810</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="C26" s="1" t="n">
-        <v>42898</v>
+        <v>42789</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="C27" s="1" t="n">
-        <v>42810</v>
+        <v>42782</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="C28" s="1" t="n">
-        <v>42789</v>
+        <v>42814</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
+        <v>9</v>
+      </c>
+      <c r="C29" s="1" t="n">
+        <v>42810</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="1" t="n">
+        <v>42808</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="1" t="n">
+        <v>42806</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="1" t="n">
+        <v>42796</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" s="1" t="n">
+        <v>42776</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C34" s="1" t="n">
+        <v>42777</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1005,110 +1206,110 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>69</v>
+        <v>90</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>